<commit_message>
excel autofit "Name" column
</commit_message>
<xml_diff>
--- a/tasklist.xlsx
+++ b/tasklist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -74,7 +74,7 @@
     <t>java.exe</t>
   </si>
   <si>
-    <t>6744</t>
+    <t>1456</t>
   </si>
   <si>
     <t>SearchIndexer.exe</t>
@@ -125,106 +125,118 @@
     <t>3304</t>
   </si>
   <si>
+    <t>OSPPSVC.EXE</t>
+  </si>
+  <si>
+    <t>8100</t>
+  </si>
+  <si>
+    <t>RuntimeBroker.exe</t>
+  </si>
+  <si>
+    <t>2196</t>
+  </si>
+  <si>
+    <t>csrss.exe</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>lsass.exe</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>audiodg.exe</t>
+  </si>
+  <si>
+    <t>7760</t>
+  </si>
+  <si>
+    <t>spd.exe</t>
+  </si>
+  <si>
+    <t>1588</t>
+  </si>
+  <si>
+    <t>cfosspeed.exe</t>
+  </si>
+  <si>
+    <t>584</t>
+  </si>
+  <si>
+    <t>dasHost.exe</t>
+  </si>
+  <si>
+    <t>2968</t>
+  </si>
+  <si>
+    <t>WmiPrvSE.exe</t>
+  </si>
+  <si>
+    <t>4088</t>
+  </si>
+  <si>
+    <t>SearchProtocolHost.exe</t>
+  </si>
+  <si>
+    <t>4752</t>
+  </si>
+  <si>
+    <t>MpCmdRun.exe</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>4game-service.exe</t>
+  </si>
+  <si>
+    <t>1484</t>
+  </si>
+  <si>
+    <t>iSCTAgent.exe</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>CCC.exe</t>
+  </si>
+  <si>
+    <t>4684</t>
+  </si>
+  <si>
+    <t>conhost.exe</t>
+  </si>
+  <si>
+    <t>7424</t>
+  </si>
+  <si>
+    <t>RAVCpl64.exe</t>
+  </si>
+  <si>
+    <t>4112</t>
+  </si>
+  <si>
+    <t>jusched.exe</t>
+  </si>
+  <si>
+    <t>4328</t>
+  </si>
+  <si>
     <t>SearchFilterHost.exe</t>
   </si>
   <si>
-    <t>8188</t>
-  </si>
-  <si>
-    <t>OSPPSVC.EXE</t>
-  </si>
-  <si>
-    <t>8100</t>
-  </si>
-  <si>
-    <t>RuntimeBroker.exe</t>
-  </si>
-  <si>
-    <t>2196</t>
-  </si>
-  <si>
-    <t>csrss.exe</t>
-  </si>
-  <si>
-    <t>496</t>
-  </si>
-  <si>
-    <t>lsass.exe</t>
-  </si>
-  <si>
-    <t>684</t>
-  </si>
-  <si>
-    <t>spd.exe</t>
-  </si>
-  <si>
-    <t>1588</t>
-  </si>
-  <si>
-    <t>cfosspeed.exe</t>
-  </si>
-  <si>
-    <t>584</t>
-  </si>
-  <si>
-    <t>dasHost.exe</t>
-  </si>
-  <si>
-    <t>2968</t>
-  </si>
-  <si>
-    <t>SearchProtocolHost.exe</t>
-  </si>
-  <si>
-    <t>3668</t>
-  </si>
-  <si>
-    <t>WmiPrvSE.exe</t>
-  </si>
-  <si>
-    <t>4088</t>
-  </si>
-  <si>
-    <t>MpCmdRun.exe</t>
-  </si>
-  <si>
-    <t>4800</t>
-  </si>
-  <si>
-    <t>4game-service.exe</t>
-  </si>
-  <si>
-    <t>1484</t>
-  </si>
-  <si>
-    <t>iSCTAgent.exe</t>
-  </si>
-  <si>
-    <t>1220</t>
-  </si>
-  <si>
-    <t>CCC.exe</t>
-  </si>
-  <si>
-    <t>4684</t>
-  </si>
-  <si>
-    <t>conhost.exe</t>
-  </si>
-  <si>
-    <t>8068</t>
-  </si>
-  <si>
-    <t>RAVCpl64.exe</t>
-  </si>
-  <si>
-    <t>4112</t>
-  </si>
-  <si>
-    <t>jusched.exe</t>
-  </si>
-  <si>
-    <t>4328</t>
+    <t>4796</t>
+  </si>
+  <si>
+    <t>NisSrv.exe</t>
+  </si>
+  <si>
+    <t>4400</t>
   </si>
   <si>
     <t>MOM.exe</t>
@@ -239,12 +251,6 @@
     <t>1308</t>
   </si>
   <si>
-    <t>NisSrv.exe</t>
-  </si>
-  <si>
-    <t>4400</t>
-  </si>
-  <si>
     <t>LMS.exe</t>
   </si>
   <si>
@@ -254,19 +260,19 @@
     <t>tasklist.exe</t>
   </si>
   <si>
-    <t>7496</t>
+    <t>6012</t>
+  </si>
+  <si>
+    <t>services.exe</t>
+  </si>
+  <si>
+    <t>656</t>
   </si>
   <si>
     <t>mdm.exe</t>
   </si>
   <si>
     <t>1604</t>
-  </si>
-  <si>
-    <t>services.exe</t>
-  </si>
-  <si>
-    <t>656</t>
   </si>
   <si>
     <t>atieclxx.exe</t>
@@ -438,112 +444,112 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$61</c:f>
+              <c:f>Sheet1!$A$2:$A$62</c:f>
               <c:numCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="61"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$61</c:f>
+              <c:f>Sheet1!$C$2:$C$62</c:f>
               <c:numCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>4122976.0</c:v>
+                  <c:v>4264972.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217556.0</c:v>
+                  <c:v>1228664.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>261260.0</c:v>
+                  <c:v>263028.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128344.0</c:v>
+                  <c:v>128356.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120080.0</c:v>
+                  <c:v>120380.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111140.0</c:v>
+                  <c:v>111208.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97576.0</c:v>
+                  <c:v>99720.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79024.0</c:v>
+                  <c:v>78348.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44948.0</c:v>
+                  <c:v>44896.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33556.0</c:v>
+                  <c:v>33460.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32772.0</c:v>
+                  <c:v>32776.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30136.0</c:v>
+                  <c:v>29240.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27316.0</c:v>
+                  <c:v>27668.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>26256.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24420.0</c:v>
+                  <c:v>24424.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16828.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16660.0</c:v>
+                  <c:v>16628.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12548.0</c:v>
+                  <c:v>11868.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11868.0</c:v>
+                  <c:v>11496.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11496.0</c:v>
+                  <c:v>11224.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11284.0</c:v>
+                  <c:v>10892.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10952.0</c:v>
+                  <c:v>10748.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10404.0</c:v>
+                  <c:v>10416.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9180.0</c:v>
+                  <c:v>9184.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>9092.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8816.0</c:v>
+                  <c:v>8784.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8600.0</c:v>
+                  <c:v>8708.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8476.0</c:v>
+                  <c:v>8464.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8308.0</c:v>
+                  <c:v>8368.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>7764.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7640.0</c:v>
+                  <c:v>7648.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6996.0</c:v>
+                  <c:v>6976.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>6936.0</c:v>
@@ -552,81 +558,84 @@
                   <c:v>6856.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6512.0</c:v>
+                  <c:v>6684.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>6548.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6528.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>6072.0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>5976.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>5876.0</c:v>
                 </c:pt>
-                <c:pt idx="38">
-                  <c:v>5816.0</c:v>
-                </c:pt>
                 <c:pt idx="39">
+                  <c:v>5820.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5772.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>5740.0</c:v>
                 </c:pt>
-                <c:pt idx="40">
-                  <c:v>5696.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>5584.0</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>4996.0</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>4604.0</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>4184.0</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>4164.0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>4112.0</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>4008.0</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3580.0</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>3428.0</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="51">
                   <c:v>3380.0</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="52">
                   <c:v>3304.0</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="53">
                   <c:v>3124.0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="54">
                   <c:v>3116.0</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="55">
                   <c:v>2940.0</c:v>
                 </c:pt>
-                <c:pt idx="55">
-                  <c:v>1832.0</c:v>
-                </c:pt>
                 <c:pt idx="56">
+                  <c:v>1792.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>848.0</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="58">
                   <c:v>572.0</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>528.0</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -720,6 +729,9 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="45.37109375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -740,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4122976.0</v>
+        <v>4264972.0</v>
       </c>
     </row>
     <row r="3">
@@ -751,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1217556.0</v>
+        <v>1228664.0</v>
       </c>
     </row>
     <row r="4">
@@ -762,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>261260.0</v>
+        <v>263028.0</v>
       </c>
     </row>
     <row r="5">
@@ -773,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>128344.0</v>
+        <v>128356.0</v>
       </c>
     </row>
     <row r="6">
@@ -784,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>120080.0</v>
+        <v>120380.0</v>
       </c>
     </row>
     <row r="7">
@@ -795,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>111140.0</v>
+        <v>111208.0</v>
       </c>
     </row>
     <row r="8">
@@ -806,7 +818,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>97576.0</v>
+        <v>99720.0</v>
       </c>
     </row>
     <row r="9">
@@ -817,7 +829,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>79024.0</v>
+        <v>78348.0</v>
       </c>
     </row>
     <row r="10">
@@ -828,7 +840,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>44948.0</v>
+        <v>44896.0</v>
       </c>
     </row>
     <row r="11">
@@ -839,7 +851,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>33556.0</v>
+        <v>33460.0</v>
       </c>
     </row>
     <row r="12">
@@ -850,7 +862,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="n">
-        <v>32772.0</v>
+        <v>32776.0</v>
       </c>
     </row>
     <row r="13">
@@ -861,7 +873,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="n">
-        <v>30136.0</v>
+        <v>29240.0</v>
       </c>
     </row>
     <row r="14">
@@ -872,7 +884,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="n">
-        <v>27316.0</v>
+        <v>27668.0</v>
       </c>
     </row>
     <row r="15">
@@ -894,7 +906,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="n">
-        <v>24420.0</v>
+        <v>24424.0</v>
       </c>
     </row>
     <row r="17">
@@ -916,7 +928,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="n">
-        <v>16660.0</v>
+        <v>16628.0</v>
       </c>
     </row>
     <row r="19">
@@ -927,7 +939,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="n">
-        <v>12548.0</v>
+        <v>11868.0</v>
       </c>
     </row>
     <row r="20">
@@ -938,7 +950,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="n">
-        <v>11868.0</v>
+        <v>11496.0</v>
       </c>
     </row>
     <row r="21">
@@ -949,7 +961,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="n">
-        <v>11496.0</v>
+        <v>11224.0</v>
       </c>
     </row>
     <row r="22">
@@ -960,7 +972,7 @@
         <v>44</v>
       </c>
       <c r="C22" t="n">
-        <v>11284.0</v>
+        <v>10892.0</v>
       </c>
     </row>
     <row r="23">
@@ -971,7 +983,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="n">
-        <v>10952.0</v>
+        <v>10748.0</v>
       </c>
     </row>
     <row r="24">
@@ -982,7 +994,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="n">
-        <v>10404.0</v>
+        <v>10416.0</v>
       </c>
     </row>
     <row r="25">
@@ -993,7 +1005,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>9180.0</v>
+        <v>9184.0</v>
       </c>
     </row>
     <row r="26">
@@ -1015,7 +1027,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="n">
-        <v>8816.0</v>
+        <v>8784.0</v>
       </c>
     </row>
     <row r="28">
@@ -1026,7 +1038,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="n">
-        <v>8600.0</v>
+        <v>8708.0</v>
       </c>
     </row>
     <row r="29">
@@ -1037,7 +1049,7 @@
         <v>58</v>
       </c>
       <c r="C29" t="n">
-        <v>8476.0</v>
+        <v>8464.0</v>
       </c>
     </row>
     <row r="30">
@@ -1048,7 +1060,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="n">
-        <v>8308.0</v>
+        <v>8368.0</v>
       </c>
     </row>
     <row r="31">
@@ -1070,7 +1082,7 @@
         <v>64</v>
       </c>
       <c r="C32" t="n">
-        <v>7640.0</v>
+        <v>7648.0</v>
       </c>
     </row>
     <row r="33">
@@ -1081,7 +1093,7 @@
         <v>66</v>
       </c>
       <c r="C33" t="n">
-        <v>6996.0</v>
+        <v>6976.0</v>
       </c>
     </row>
     <row r="34">
@@ -1114,7 +1126,7 @@
         <v>72</v>
       </c>
       <c r="C36" t="n">
-        <v>6512.0</v>
+        <v>6684.0</v>
       </c>
     </row>
     <row r="37">
@@ -1125,7 +1137,7 @@
         <v>74</v>
       </c>
       <c r="C37" t="n">
-        <v>6072.0</v>
+        <v>6548.0</v>
       </c>
     </row>
     <row r="38">
@@ -1136,7 +1148,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="n">
-        <v>5976.0</v>
+        <v>6528.0</v>
       </c>
     </row>
     <row r="39">
@@ -1147,7 +1159,7 @@
         <v>78</v>
       </c>
       <c r="C39" t="n">
-        <v>5876.0</v>
+        <v>6072.0</v>
       </c>
     </row>
     <row r="40">
@@ -1158,7 +1170,7 @@
         <v>80</v>
       </c>
       <c r="C40" t="n">
-        <v>5816.0</v>
+        <v>5876.0</v>
       </c>
     </row>
     <row r="41">
@@ -1169,7 +1181,7 @@
         <v>82</v>
       </c>
       <c r="C41" t="n">
-        <v>5740.0</v>
+        <v>5820.0</v>
       </c>
     </row>
     <row r="42">
@@ -1180,7 +1192,7 @@
         <v>84</v>
       </c>
       <c r="C42" t="n">
-        <v>5696.0</v>
+        <v>5772.0</v>
       </c>
     </row>
     <row r="43">
@@ -1191,7 +1203,7 @@
         <v>86</v>
       </c>
       <c r="C43" t="n">
-        <v>5584.0</v>
+        <v>5740.0</v>
       </c>
     </row>
     <row r="44">
@@ -1202,7 +1214,7 @@
         <v>88</v>
       </c>
       <c r="C44" t="n">
-        <v>4996.0</v>
+        <v>5584.0</v>
       </c>
     </row>
     <row r="45">
@@ -1213,7 +1225,7 @@
         <v>90</v>
       </c>
       <c r="C45" t="n">
-        <v>4604.0</v>
+        <v>4996.0</v>
       </c>
     </row>
     <row r="46">
@@ -1224,7 +1236,7 @@
         <v>92</v>
       </c>
       <c r="C46" t="n">
-        <v>4184.0</v>
+        <v>4604.0</v>
       </c>
     </row>
     <row r="47">
@@ -1235,7 +1247,7 @@
         <v>94</v>
       </c>
       <c r="C47" t="n">
-        <v>4164.0</v>
+        <v>4184.0</v>
       </c>
     </row>
     <row r="48">
@@ -1246,7 +1258,7 @@
         <v>96</v>
       </c>
       <c r="C48" t="n">
-        <v>4112.0</v>
+        <v>4164.0</v>
       </c>
     </row>
     <row r="49">
@@ -1257,7 +1269,7 @@
         <v>98</v>
       </c>
       <c r="C49" t="n">
-        <v>4008.0</v>
+        <v>4112.0</v>
       </c>
     </row>
     <row r="50">
@@ -1268,7 +1280,7 @@
         <v>100</v>
       </c>
       <c r="C50" t="n">
-        <v>3580.0</v>
+        <v>4008.0</v>
       </c>
     </row>
     <row r="51">
@@ -1279,7 +1291,7 @@
         <v>102</v>
       </c>
       <c r="C51" t="n">
-        <v>3428.0</v>
+        <v>3580.0</v>
       </c>
     </row>
     <row r="52">
@@ -1290,7 +1302,7 @@
         <v>104</v>
       </c>
       <c r="C52" t="n">
-        <v>3380.0</v>
+        <v>3428.0</v>
       </c>
     </row>
     <row r="53">
@@ -1301,7 +1313,7 @@
         <v>106</v>
       </c>
       <c r="C53" t="n">
-        <v>3304.0</v>
+        <v>3380.0</v>
       </c>
     </row>
     <row r="54">
@@ -1312,7 +1324,7 @@
         <v>108</v>
       </c>
       <c r="C54" t="n">
-        <v>3124.0</v>
+        <v>3304.0</v>
       </c>
     </row>
     <row r="55">
@@ -1323,7 +1335,7 @@
         <v>110</v>
       </c>
       <c r="C55" t="n">
-        <v>3116.0</v>
+        <v>3124.0</v>
       </c>
     </row>
     <row r="56">
@@ -1334,7 +1346,7 @@
         <v>112</v>
       </c>
       <c r="C56" t="n">
-        <v>2940.0</v>
+        <v>3116.0</v>
       </c>
     </row>
     <row r="57">
@@ -1345,7 +1357,7 @@
         <v>114</v>
       </c>
       <c r="C57" t="n">
-        <v>1832.0</v>
+        <v>2940.0</v>
       </c>
     </row>
     <row r="58">
@@ -1356,7 +1368,7 @@
         <v>116</v>
       </c>
       <c r="C58" t="n">
-        <v>848.0</v>
+        <v>1792.0</v>
       </c>
     </row>
     <row r="59">
@@ -1367,7 +1379,7 @@
         <v>118</v>
       </c>
       <c r="C59" t="n">
-        <v>572.0</v>
+        <v>848.0</v>
       </c>
     </row>
     <row r="60">
@@ -1378,7 +1390,7 @@
         <v>120</v>
       </c>
       <c r="C60" t="n">
-        <v>528.0</v>
+        <v>572.0</v>
       </c>
     </row>
     <row r="61">
@@ -1389,6 +1401,17 @@
         <v>122</v>
       </c>
       <c r="C61" t="n">
+        <v>528.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" t="n">
         <v>4.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
load from file #6 fix
</commit_message>
<xml_diff>
--- a/tasklist.xlsx
+++ b/tasklist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +41,18 @@
     <t>756</t>
   </si>
   <si>
+    <t>java.exe</t>
+  </si>
+  <si>
+    <t>732</t>
+  </si>
+  <si>
+    <t>MsMpEng.exe</t>
+  </si>
+  <si>
+    <t>2260</t>
+  </si>
+  <si>
     <t>Skype.exe</t>
   </si>
   <si>
@@ -53,12 +65,6 @@
     <t>5728</t>
   </si>
   <si>
-    <t>MsMpEng.exe</t>
-  </si>
-  <si>
-    <t>2260</t>
-  </si>
-  <si>
     <t>ekrn.exe</t>
   </si>
   <si>
@@ -71,12 +77,6 @@
     <t>3256</t>
   </si>
   <si>
-    <t>java.exe</t>
-  </si>
-  <si>
-    <t>1456</t>
-  </si>
-  <si>
     <t>SearchIndexer.exe</t>
   </si>
   <si>
@@ -101,18 +101,18 @@
     <t>1748</t>
   </si>
   <si>
+    <t>egui.exe</t>
+  </si>
+  <si>
+    <t>3296</t>
+  </si>
+  <si>
     <t>IAStorDataMgrSvc.exe</t>
   </si>
   <si>
     <t>3960</t>
   </si>
   <si>
-    <t>egui.exe</t>
-  </si>
-  <si>
-    <t>3296</t>
-  </si>
-  <si>
     <t>IAStorIcon.exe</t>
   </si>
   <si>
@@ -152,7 +152,7 @@
     <t>audiodg.exe</t>
   </si>
   <si>
-    <t>7760</t>
+    <t>7636</t>
   </si>
   <si>
     <t>spd.exe</t>
@@ -161,6 +161,12 @@
     <t>1588</t>
   </si>
   <si>
+    <t>WmiPrvSE.exe</t>
+  </si>
+  <si>
+    <t>4088</t>
+  </si>
+  <si>
     <t>cfosspeed.exe</t>
   </si>
   <si>
@@ -173,190 +179,190 @@
     <t>2968</t>
   </si>
   <si>
-    <t>WmiPrvSE.exe</t>
-  </si>
-  <si>
-    <t>4088</t>
+    <t>taskhost.exe</t>
+  </si>
+  <si>
+    <t>5768</t>
+  </si>
+  <si>
+    <t>MpCmdRun.exe</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>4game-service.exe</t>
+  </si>
+  <si>
+    <t>1484</t>
+  </si>
+  <si>
+    <t>CCC.exe</t>
+  </si>
+  <si>
+    <t>4684</t>
+  </si>
+  <si>
+    <t>iSCTAgent.exe</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>RAVCpl64.exe</t>
+  </si>
+  <si>
+    <t>4112</t>
+  </si>
+  <si>
+    <t>conhost.exe</t>
+  </si>
+  <si>
+    <t>1040</t>
+  </si>
+  <si>
+    <t>jusched.exe</t>
+  </si>
+  <si>
+    <t>4328</t>
+  </si>
+  <si>
+    <t>atieclxx.exe</t>
+  </si>
+  <si>
+    <t>2808</t>
+  </si>
+  <si>
+    <t>spoolsv.exe</t>
+  </si>
+  <si>
+    <t>1308</t>
+  </si>
+  <si>
+    <t>MOM.exe</t>
+  </si>
+  <si>
+    <t>4320</t>
+  </si>
+  <si>
+    <t>services.exe</t>
+  </si>
+  <si>
+    <t>656</t>
+  </si>
+  <si>
+    <t>LMS.exe</t>
+  </si>
+  <si>
+    <t>3532</t>
+  </si>
+  <si>
+    <t>tasklist.exe</t>
+  </si>
+  <si>
+    <t>4796</t>
+  </si>
+  <si>
+    <t>mdm.exe</t>
+  </si>
+  <si>
+    <t>1604</t>
   </si>
   <si>
     <t>SearchProtocolHost.exe</t>
   </si>
   <si>
-    <t>4752</t>
-  </si>
-  <si>
-    <t>MpCmdRun.exe</t>
-  </si>
-  <si>
-    <t>4800</t>
-  </si>
-  <si>
-    <t>4game-service.exe</t>
-  </si>
-  <si>
-    <t>1484</t>
-  </si>
-  <si>
-    <t>iSCTAgent.exe</t>
-  </si>
-  <si>
-    <t>1220</t>
-  </si>
-  <si>
-    <t>CCC.exe</t>
-  </si>
-  <si>
-    <t>4684</t>
-  </si>
-  <si>
-    <t>conhost.exe</t>
-  </si>
-  <si>
-    <t>7424</t>
-  </si>
-  <si>
-    <t>RAVCpl64.exe</t>
-  </si>
-  <si>
-    <t>4112</t>
-  </si>
-  <si>
-    <t>jusched.exe</t>
-  </si>
-  <si>
-    <t>4328</t>
+    <t>7504</t>
+  </si>
+  <si>
+    <t>winlogon.exe</t>
+  </si>
+  <si>
+    <t>648</t>
   </si>
   <si>
     <t>SearchFilterHost.exe</t>
   </si>
   <si>
-    <t>4796</t>
+    <t>3112</t>
+  </si>
+  <si>
+    <t>slimsvc.exe</t>
+  </si>
+  <si>
+    <t>1616</t>
+  </si>
+  <si>
+    <t>WUDFHost.exe</t>
+  </si>
+  <si>
+    <t>2980</t>
+  </si>
+  <si>
+    <t>iSCTsysTray8.exe</t>
+  </si>
+  <si>
+    <t>876</t>
+  </si>
+  <si>
+    <t>sqlwriter.exe</t>
+  </si>
+  <si>
+    <t>2168</t>
+  </si>
+  <si>
+    <t>IPROSetMonitor.exe</t>
+  </si>
+  <si>
+    <t>1232</t>
+  </si>
+  <si>
+    <t>IOMonitorSrv.exe</t>
+  </si>
+  <si>
+    <t>1568</t>
+  </si>
+  <si>
+    <t>jhi_service.exe</t>
+  </si>
+  <si>
+    <t>1472</t>
+  </si>
+  <si>
+    <t>SbieSvc.exe</t>
+  </si>
+  <si>
+    <t>1032</t>
+  </si>
+  <si>
+    <t>atiesrxx.exe</t>
+  </si>
+  <si>
+    <t>964</t>
+  </si>
+  <si>
+    <t>IntelMeFWService.exe</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>wininit.exe</t>
+  </si>
+  <si>
+    <t>572</t>
+  </si>
+  <si>
+    <t>Start8_64.exe</t>
+  </si>
+  <si>
+    <t>1156</t>
   </si>
   <si>
     <t>NisSrv.exe</t>
   </si>
   <si>
     <t>4400</t>
-  </si>
-  <si>
-    <t>MOM.exe</t>
-  </si>
-  <si>
-    <t>4320</t>
-  </si>
-  <si>
-    <t>spoolsv.exe</t>
-  </si>
-  <si>
-    <t>1308</t>
-  </si>
-  <si>
-    <t>LMS.exe</t>
-  </si>
-  <si>
-    <t>3532</t>
-  </si>
-  <si>
-    <t>tasklist.exe</t>
-  </si>
-  <si>
-    <t>6012</t>
-  </si>
-  <si>
-    <t>services.exe</t>
-  </si>
-  <si>
-    <t>656</t>
-  </si>
-  <si>
-    <t>mdm.exe</t>
-  </si>
-  <si>
-    <t>1604</t>
-  </si>
-  <si>
-    <t>atieclxx.exe</t>
-  </si>
-  <si>
-    <t>2808</t>
-  </si>
-  <si>
-    <t>winlogon.exe</t>
-  </si>
-  <si>
-    <t>648</t>
-  </si>
-  <si>
-    <t>slimsvc.exe</t>
-  </si>
-  <si>
-    <t>1616</t>
-  </si>
-  <si>
-    <t>sqlwriter.exe</t>
-  </si>
-  <si>
-    <t>2168</t>
-  </si>
-  <si>
-    <t>iSCTsysTray8.exe</t>
-  </si>
-  <si>
-    <t>876</t>
-  </si>
-  <si>
-    <t>IPROSetMonitor.exe</t>
-  </si>
-  <si>
-    <t>1232</t>
-  </si>
-  <si>
-    <t>WUDFHost.exe</t>
-  </si>
-  <si>
-    <t>2980</t>
-  </si>
-  <si>
-    <t>IOMonitorSrv.exe</t>
-  </si>
-  <si>
-    <t>1568</t>
-  </si>
-  <si>
-    <t>jhi_service.exe</t>
-  </si>
-  <si>
-    <t>1472</t>
-  </si>
-  <si>
-    <t>SbieSvc.exe</t>
-  </si>
-  <si>
-    <t>1032</t>
-  </si>
-  <si>
-    <t>atiesrxx.exe</t>
-  </si>
-  <si>
-    <t>964</t>
-  </si>
-  <si>
-    <t>IntelMeFWService.exe</t>
-  </si>
-  <si>
-    <t>1600</t>
-  </si>
-  <si>
-    <t>wininit.exe</t>
-  </si>
-  <si>
-    <t>572</t>
-  </si>
-  <si>
-    <t>Start8_64.exe</t>
-  </si>
-  <si>
-    <t>1156</t>
   </si>
   <si>
     <t>System</t>
@@ -444,163 +450,163 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$62</c:f>
+              <c:f>Sheet1!$A$2:$A$63</c:f>
               <c:numCache>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$62</c:f>
+              <c:f>Sheet1!$C$2:$C$63</c:f>
               <c:numCache>
-                <c:ptCount val="61"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>4264972.0</c:v>
+                  <c:v>4263844.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1228664.0</c:v>
+                  <c:v>1622600.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>263028.0</c:v>
+                  <c:v>274340.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128356.0</c:v>
+                  <c:v>162572.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120380.0</c:v>
+                  <c:v>135400.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111208.0</c:v>
+                  <c:v>129888.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>99720.0</c:v>
+                  <c:v>121872.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78348.0</c:v>
+                  <c:v>101536.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44896.0</c:v>
+                  <c:v>81228.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33460.0</c:v>
+                  <c:v>39128.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32776.0</c:v>
+                  <c:v>36272.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29240.0</c:v>
+                  <c:v>32864.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27668.0</c:v>
+                  <c:v>31460.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26256.0</c:v>
+                  <c:v>25380.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24424.0</c:v>
+                  <c:v>24832.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16828.0</c:v>
+                  <c:v>17160.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16628.0</c:v>
+                  <c:v>15424.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>11868.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11496.0</c:v>
+                  <c:v>11624.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11224.0</c:v>
+                  <c:v>11612.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10892.0</c:v>
+                  <c:v>11376.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10748.0</c:v>
+                  <c:v>10732.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10416.0</c:v>
+                  <c:v>10368.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9184.0</c:v>
+                  <c:v>10064.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>9360.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>9092.0</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>8784.0</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>8708.0</c:v>
+                  <c:v>9060.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8464.0</c:v>
+                  <c:v>8644.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8368.0</c:v>
+                  <c:v>8340.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>7780.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>7764.0</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>7648.0</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>6976.0</c:v>
+                  <c:v>7060.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6936.0</c:v>
+                  <c:v>7004.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6856.0</c:v>
+                  <c:v>6888.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6684.0</c:v>
+                  <c:v>6292.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6548.0</c:v>
+                  <c:v>6072.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6528.0</c:v>
+                  <c:v>6008.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6072.0</c:v>
+                  <c:v>5956.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>5876.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5820.0</c:v>
+                  <c:v>5816.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5772.0</c:v>
+                  <c:v>5756.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5740.0</c:v>
+                  <c:v>5104.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5584.0</c:v>
+                  <c:v>5080.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4996.0</c:v>
+                  <c:v>4988.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>4604.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>4376.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4224.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>4184.0</c:v>
                 </c:pt>
-                <c:pt idx="46">
-                  <c:v>4164.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>4112.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4008.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>3580.0</c:v>
@@ -612,7 +618,7 @@
                   <c:v>3380.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3304.0</c:v>
+                  <c:v>3340.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>3124.0</c:v>
@@ -621,21 +627,24 @@
                   <c:v>3116.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2940.0</c:v>
+                  <c:v>3020.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1792.0</c:v>
+                  <c:v>2624.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
+                  <c:v>2492.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>848.0</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="59">
                   <c:v>572.0</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="60">
                   <c:v>528.0</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="61">
                   <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -752,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4264972.0</v>
+        <v>4263844.0</v>
       </c>
     </row>
     <row r="3">
@@ -763,7 +772,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1228664.0</v>
+        <v>1622600.0</v>
       </c>
     </row>
     <row r="4">
@@ -774,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>263028.0</v>
+        <v>274340.0</v>
       </c>
     </row>
     <row r="5">
@@ -785,7 +794,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>128356.0</v>
+        <v>162572.0</v>
       </c>
     </row>
     <row r="6">
@@ -796,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>120380.0</v>
+        <v>135400.0</v>
       </c>
     </row>
     <row r="7">
@@ -807,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>111208.0</v>
+        <v>129888.0</v>
       </c>
     </row>
     <row r="8">
@@ -818,7 +827,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>99720.0</v>
+        <v>121872.0</v>
       </c>
     </row>
     <row r="9">
@@ -829,7 +838,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>78348.0</v>
+        <v>101536.0</v>
       </c>
     </row>
     <row r="10">
@@ -840,7 +849,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>44896.0</v>
+        <v>81228.0</v>
       </c>
     </row>
     <row r="11">
@@ -851,7 +860,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>33460.0</v>
+        <v>39128.0</v>
       </c>
     </row>
     <row r="12">
@@ -862,7 +871,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="n">
-        <v>32776.0</v>
+        <v>36272.0</v>
       </c>
     </row>
     <row r="13">
@@ -873,7 +882,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="n">
-        <v>29240.0</v>
+        <v>32864.0</v>
       </c>
     </row>
     <row r="14">
@@ -884,7 +893,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="n">
-        <v>27668.0</v>
+        <v>31460.0</v>
       </c>
     </row>
     <row r="15">
@@ -895,7 +904,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>26256.0</v>
+        <v>25380.0</v>
       </c>
     </row>
     <row r="16">
@@ -906,7 +915,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="n">
-        <v>24424.0</v>
+        <v>24832.0</v>
       </c>
     </row>
     <row r="17">
@@ -917,7 +926,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="n">
-        <v>16828.0</v>
+        <v>17160.0</v>
       </c>
     </row>
     <row r="18">
@@ -928,7 +937,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="n">
-        <v>16628.0</v>
+        <v>15424.0</v>
       </c>
     </row>
     <row r="19">
@@ -950,7 +959,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="n">
-        <v>11496.0</v>
+        <v>11624.0</v>
       </c>
     </row>
     <row r="21">
@@ -961,7 +970,7 @@
         <v>42</v>
       </c>
       <c r="C21" t="n">
-        <v>11224.0</v>
+        <v>11612.0</v>
       </c>
     </row>
     <row r="22">
@@ -972,7 +981,7 @@
         <v>44</v>
       </c>
       <c r="C22" t="n">
-        <v>10892.0</v>
+        <v>11376.0</v>
       </c>
     </row>
     <row r="23">
@@ -983,7 +992,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="n">
-        <v>10748.0</v>
+        <v>10732.0</v>
       </c>
     </row>
     <row r="24">
@@ -994,7 +1003,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="n">
-        <v>10416.0</v>
+        <v>10368.0</v>
       </c>
     </row>
     <row r="25">
@@ -1005,7 +1014,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>9184.0</v>
+        <v>10064.0</v>
       </c>
     </row>
     <row r="26">
@@ -1016,7 +1025,7 @@
         <v>52</v>
       </c>
       <c r="C26" t="n">
-        <v>9092.0</v>
+        <v>9360.0</v>
       </c>
     </row>
     <row r="27">
@@ -1027,7 +1036,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="n">
-        <v>8784.0</v>
+        <v>9092.0</v>
       </c>
     </row>
     <row r="28">
@@ -1038,7 +1047,7 @@
         <v>56</v>
       </c>
       <c r="C28" t="n">
-        <v>8708.0</v>
+        <v>9060.0</v>
       </c>
     </row>
     <row r="29">
@@ -1049,7 +1058,7 @@
         <v>58</v>
       </c>
       <c r="C29" t="n">
-        <v>8464.0</v>
+        <v>8644.0</v>
       </c>
     </row>
     <row r="30">
@@ -1060,7 +1069,7 @@
         <v>60</v>
       </c>
       <c r="C30" t="n">
-        <v>8368.0</v>
+        <v>8340.0</v>
       </c>
     </row>
     <row r="31">
@@ -1071,7 +1080,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="n">
-        <v>7764.0</v>
+        <v>7780.0</v>
       </c>
     </row>
     <row r="32">
@@ -1082,7 +1091,7 @@
         <v>64</v>
       </c>
       <c r="C32" t="n">
-        <v>7648.0</v>
+        <v>7764.0</v>
       </c>
     </row>
     <row r="33">
@@ -1093,7 +1102,7 @@
         <v>66</v>
       </c>
       <c r="C33" t="n">
-        <v>6976.0</v>
+        <v>7060.0</v>
       </c>
     </row>
     <row r="34">
@@ -1104,7 +1113,7 @@
         <v>68</v>
       </c>
       <c r="C34" t="n">
-        <v>6936.0</v>
+        <v>7004.0</v>
       </c>
     </row>
     <row r="35">
@@ -1115,7 +1124,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="n">
-        <v>6856.0</v>
+        <v>6888.0</v>
       </c>
     </row>
     <row r="36">
@@ -1126,7 +1135,7 @@
         <v>72</v>
       </c>
       <c r="C36" t="n">
-        <v>6684.0</v>
+        <v>6292.0</v>
       </c>
     </row>
     <row r="37">
@@ -1137,7 +1146,7 @@
         <v>74</v>
       </c>
       <c r="C37" t="n">
-        <v>6548.0</v>
+        <v>6072.0</v>
       </c>
     </row>
     <row r="38">
@@ -1148,7 +1157,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="n">
-        <v>6528.0</v>
+        <v>6008.0</v>
       </c>
     </row>
     <row r="39">
@@ -1159,7 +1168,7 @@
         <v>78</v>
       </c>
       <c r="C39" t="n">
-        <v>6072.0</v>
+        <v>5956.0</v>
       </c>
     </row>
     <row r="40">
@@ -1181,7 +1190,7 @@
         <v>82</v>
       </c>
       <c r="C41" t="n">
-        <v>5820.0</v>
+        <v>5816.0</v>
       </c>
     </row>
     <row r="42">
@@ -1192,7 +1201,7 @@
         <v>84</v>
       </c>
       <c r="C42" t="n">
-        <v>5772.0</v>
+        <v>5756.0</v>
       </c>
     </row>
     <row r="43">
@@ -1203,7 +1212,7 @@
         <v>86</v>
       </c>
       <c r="C43" t="n">
-        <v>5740.0</v>
+        <v>5104.0</v>
       </c>
     </row>
     <row r="44">
@@ -1214,7 +1223,7 @@
         <v>88</v>
       </c>
       <c r="C44" t="n">
-        <v>5584.0</v>
+        <v>5080.0</v>
       </c>
     </row>
     <row r="45">
@@ -1225,7 +1234,7 @@
         <v>90</v>
       </c>
       <c r="C45" t="n">
-        <v>4996.0</v>
+        <v>4988.0</v>
       </c>
     </row>
     <row r="46">
@@ -1247,7 +1256,7 @@
         <v>94</v>
       </c>
       <c r="C47" t="n">
-        <v>4184.0</v>
+        <v>4376.0</v>
       </c>
     </row>
     <row r="48">
@@ -1258,7 +1267,7 @@
         <v>96</v>
       </c>
       <c r="C48" t="n">
-        <v>4164.0</v>
+        <v>4224.0</v>
       </c>
     </row>
     <row r="49">
@@ -1269,7 +1278,7 @@
         <v>98</v>
       </c>
       <c r="C49" t="n">
-        <v>4112.0</v>
+        <v>4184.0</v>
       </c>
     </row>
     <row r="50">
@@ -1280,7 +1289,7 @@
         <v>100</v>
       </c>
       <c r="C50" t="n">
-        <v>4008.0</v>
+        <v>4112.0</v>
       </c>
     </row>
     <row r="51">
@@ -1324,7 +1333,7 @@
         <v>108</v>
       </c>
       <c r="C54" t="n">
-        <v>3304.0</v>
+        <v>3340.0</v>
       </c>
     </row>
     <row r="55">
@@ -1357,7 +1366,7 @@
         <v>114</v>
       </c>
       <c r="C57" t="n">
-        <v>2940.0</v>
+        <v>3020.0</v>
       </c>
     </row>
     <row r="58">
@@ -1368,7 +1377,7 @@
         <v>116</v>
       </c>
       <c r="C58" t="n">
-        <v>1792.0</v>
+        <v>2624.0</v>
       </c>
     </row>
     <row r="59">
@@ -1379,7 +1388,7 @@
         <v>118</v>
       </c>
       <c r="C59" t="n">
-        <v>848.0</v>
+        <v>2492.0</v>
       </c>
     </row>
     <row r="60">
@@ -1390,7 +1399,7 @@
         <v>120</v>
       </c>
       <c r="C60" t="n">
-        <v>572.0</v>
+        <v>848.0</v>
       </c>
     </row>
     <row r="61">
@@ -1401,7 +1410,7 @@
         <v>122</v>
       </c>
       <c r="C61" t="n">
-        <v>528.0</v>
+        <v>572.0</v>
       </c>
     </row>
     <row r="62">
@@ -1412,6 +1421,17 @@
         <v>124</v>
       </c>
       <c r="C62" t="n">
+        <v>528.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" t="n">
         <v>4.0</v>
       </c>
     </row>

</xml_diff>